<commit_message>
feat(project): added mongodb data modelling sample document with eCommerce example
</commit_message>
<xml_diff>
--- a/1_Materials/class_notes.xlsx
+++ b/1_Materials/class_notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="127">
   <si>
     <t>DATABASE</t>
   </si>
@@ -195,9 +195,6 @@
     <t>insertOne, insertMany</t>
   </si>
   <si>
-    <t>find</t>
-  </si>
-  <si>
     <t>updateOne, UpdateMany</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
   </si>
   <si>
     <t>use &lt;database_name&gt;</t>
-  </si>
-  <si>
-    <t>db.collection_name.insertOne({})</t>
   </si>
   <si>
     <t>db.collection_name.find()</t>
@@ -393,18 +387,12 @@
     <t>local</t>
   </si>
   <si>
-    <t>{name: "Wireless Mouse", brand: "Dell"}</t>
-  </si>
-  <si>
     <t>updateMany</t>
   </si>
   <si>
     <t>deleteOne({filter})</t>
   </si>
   <si>
-    <t>db.collection_name.drop()</t>
-  </si>
-  <si>
     <t>db.dropDatabase()</t>
   </si>
   <si>
@@ -448,6 +436,76 @@
   </si>
   <si>
     <t>update object fields inside an array</t>
+  </si>
+  <si>
+    <t>find, findOne</t>
+  </si>
+  <si>
+    <t>MYSQL</t>
+  </si>
+  <si>
+    <t>MONGODB</t>
+  </si>
+  <si>
+    <t>_id: ObjectId()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.collection_name.insertOne({})</t>
+    </r>
+  </si>
+  <si>
+    <t>{name: "Wireless Mouse"}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.collection_name.drop()</t>
+    </r>
+  </si>
+  <si>
+    <t>add a new element - duplictes</t>
+  </si>
+  <si>
+    <t>add a new element - no duplictes</t>
+  </si>
+  <si>
+    <t>remove an element</t>
   </si>
 </sst>
 </file>
@@ -562,6 +620,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -592,14 +658,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -678,14 +736,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A14:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="rollNo" dataDxfId="6"/>
-    <tableColumn id="2" name="name" dataDxfId="5"/>
-    <tableColumn id="3" name="mobile" dataDxfId="4"/>
-    <tableColumn id="4" name="email" dataDxfId="3" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="deptNo" dataDxfId="2"/>
+    <tableColumn id="1" name="rollNo" dataDxfId="4"/>
+    <tableColumn id="2" name="name" dataDxfId="3"/>
+    <tableColumn id="3" name="mobile" dataDxfId="2"/>
+    <tableColumn id="4" name="email" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="deptNo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -956,16 +1014,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
@@ -1080,7 +1138,7 @@
       <c r="E14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1108,16 +1166,16 @@
       <c r="A16" s="4">
         <v>2</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>300</v>
       </c>
       <c r="G16" s="1">
@@ -1125,7 +1183,7 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1139,7 +1197,7 @@
     </row>
     <row r="22" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -1153,7 +1211,7 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1206,7 +1264,7 @@
         <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
@@ -1214,7 +1272,7 @@
         <v>48</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
@@ -1222,75 +1280,86 @@
         <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
-        <v>68</v>
+        <v>121</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
@@ -1300,26 +1369,26 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
@@ -1329,59 +1398,61 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C80" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="1" t="s">
+      <c r="D81" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D82" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D83" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
@@ -1391,35 +1462,35 @@
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
@@ -1429,100 +1500,109 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C97" s="1" t="s">
-        <v>98</v>
+      <c r="C97" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B108" s="2"/>
       <c r="E108" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D109" s="2"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C110" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B113" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B116" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(project-eCommerce): added all collections document
</commit_message>
<xml_diff>
--- a/1_Materials/class_notes.xlsx
+++ b/1_Materials/class_notes.xlsx
@@ -1012,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K116"/>
+  <dimension ref="A2:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,148 +1460,148 @@
         <v>49</v>
       </c>
     </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B86" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D89" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="2" t="s">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B90" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B92" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B95" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C97" s="2" t="s">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C96" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B99" s="1" t="s">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B98" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B103" s="2" t="s">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B102" s="2" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B107" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>126</v>
+      <c r="B107" s="2"/>
+      <c r="E107" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B108" s="2"/>
-      <c r="E108" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B108" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D108" s="2"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B109" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C109" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C110" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="2" t="s">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B112" s="2" t="s">
         <v>112</v>
       </c>
     </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B114" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B115" s="1" t="s">
-        <v>113</v>
+      <c r="B115" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C116" s="1" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(project): added project abstract template
</commit_message>
<xml_diff>
--- a/1_Materials/class_notes.xlsx
+++ b/1_Materials/class_notes.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="161">
   <si>
     <t>DATABASE</t>
   </si>
@@ -506,6 +507,109 @@
   </si>
   <si>
     <t>remove an element</t>
+  </si>
+  <si>
+    <t>RELATIONSHIPS</t>
+  </si>
+  <si>
+    <t>1:N</t>
+  </si>
+  <si>
+    <t>M:M</t>
+  </si>
+  <si>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>Student : Address
+College : Address</t>
+  </si>
+  <si>
+    <t>Department : Student</t>
+  </si>
+  <si>
+    <t>Project : Student</t>
+  </si>
+  <si>
+    <t>student_name</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>proj_id</t>
+  </si>
+  <si>
+    <t>proj_name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>Stage 2</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>Poj</t>
+  </si>
+  <si>
+    <t>Stage 3</t>
+  </si>
+  <si>
+    <t>either</t>
+  </si>
+  <si>
+    <t>many</t>
+  </si>
+  <si>
+    <t>separate</t>
+  </si>
+  <si>
+    <t>Emb</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>AGGREGATION</t>
+  </si>
+  <si>
+    <t>select from where groupby having order by limit offset</t>
+  </si>
+  <si>
+    <t>aggregation pipeline</t>
+  </si>
+  <si>
+    <t>stages</t>
+  </si>
+  <si>
+    <t>stage1</t>
+  </si>
+  <si>
+    <t>stage2</t>
+  </si>
+  <si>
+    <t>output1</t>
+  </si>
+  <si>
+    <t>input2</t>
+  </si>
+  <si>
+    <t>input1</t>
+  </si>
+  <si>
+    <t>output2</t>
   </si>
 </sst>
 </file>
@@ -583,7 +687,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -593,6 +697,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -746,6 +851,51 @@
     <tableColumn id="5" name="deptNo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D4:E6" totalsRowShown="0">
+  <autoFilter ref="D4:E6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="rollNo"/>
+    <tableColumn id="2" name="student_name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="H4:J6" totalsRowShown="0">
+  <autoFilter ref="H4:J6"/>
+  <tableColumns count="3">
+    <tableColumn id="3" name="proj_id"/>
+    <tableColumn id="1" name="proj_name"/>
+    <tableColumn id="2" name="status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="F9:G12" totalsRowShown="0">
+  <autoFilter ref="F9:G12">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="p1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="rollNo"/>
+    <tableColumn id="2" name="proj_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1012,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K115"/>
+  <dimension ref="A2:K139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,7 +1739,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B114" s="1" t="s">
         <v>113</v>
       </c>
@@ -1597,12 +1747,102 @@
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B118" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B124" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B125" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B135" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B138" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B139" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1616,4 +1856,115 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:J12"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(material): added html demo file, feat(practice_questions): added assignment and project instruction
</commit_message>
<xml_diff>
--- a/1_Materials/class_notes.xlsx
+++ b/1_Materials/class_notes.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="MongoDB" sheetId="1" r:id="rId1"/>
+    <sheet name="HTML" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="219">
   <si>
     <t>DATABASE</t>
   </si>
@@ -531,42 +531,6 @@
     <t>Project : Student</t>
   </si>
   <si>
-    <t>student_name</t>
-  </si>
-  <si>
-    <t>pk</t>
-  </si>
-  <si>
-    <t>proj_id</t>
-  </si>
-  <si>
-    <t>proj_name</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>AK</t>
-  </si>
-  <si>
-    <t>Stage 2</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>Poj</t>
-  </si>
-  <si>
-    <t>Stage 3</t>
-  </si>
-  <si>
     <t>either</t>
   </si>
   <si>
@@ -646,6 +610,180 @@
   </si>
   <si>
     <t>project</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>frontend</t>
+  </si>
+  <si>
+    <t>backend</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>element - inline/block</t>
+  </si>
+  <si>
+    <t>ui</t>
+  </si>
+  <si>
+    <t>rest api</t>
+  </si>
+  <si>
+    <t>mongodb atals</t>
+  </si>
+  <si>
+    <t>selectors - id, class, data</t>
+  </si>
+  <si>
+    <t>emmet</t>
+  </si>
+  <si>
+    <t>advanced tags</t>
+  </si>
+  <si>
+    <t>vercel</t>
+  </si>
+  <si>
+    <t>render</t>
+  </si>
+  <si>
+    <t>sementic tags</t>
+  </si>
+  <si>
+    <t>ELEMENTS</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>content width</t>
+  </si>
+  <si>
+    <t>full width</t>
+  </si>
+  <si>
+    <t>don’t break</t>
+  </si>
+  <si>
+    <t>start on new line</t>
+  </si>
+  <si>
+    <t>SELECTORS</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>EMMET</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>parent - child</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>siblings</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>repetition</t>
+  </si>
+  <si>
+    <t>text content</t>
+  </si>
+  <si>
+    <t>class selector</t>
+  </si>
+  <si>
+    <t>id selector</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>ADVANCED TAGS</t>
+  </si>
+  <si>
+    <t>figure</t>
+  </si>
+  <si>
+    <t>image + caption</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>accordion style</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>loading</t>
+  </si>
+  <si>
+    <t>abbr</t>
+  </si>
+  <si>
+    <t>acronyms</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>dates or events</t>
+  </si>
+  <si>
+    <t>SEMENTIC</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>nav</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>aside</t>
+  </si>
+  <si>
+    <t>footer</t>
   </si>
 </sst>
 </file>
@@ -887,51 +1025,6 @@
     <tableColumn id="5" name="deptNo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="D4:E6" totalsRowShown="0">
-  <autoFilter ref="D4:E6"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="rollNo"/>
-    <tableColumn id="2" name="student_name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="H4:J6" totalsRowShown="0">
-  <autoFilter ref="H4:J6"/>
-  <tableColumns count="3">
-    <tableColumn id="3" name="proj_id"/>
-    <tableColumn id="1" name="proj_name"/>
-    <tableColumn id="2" name="status"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="F9:G12" totalsRowShown="0">
-  <autoFilter ref="F9:G12">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="p1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="rollNo"/>
-    <tableColumn id="2" name="proj_id"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1200,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,7 +1891,7 @@
     </row>
     <row r="120" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>130</v>
@@ -1809,7 +1902,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>128</v>
@@ -1820,7 +1913,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>129</v>
@@ -1831,72 +1924,72 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B134" s="1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B138" s="1" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B139" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B142" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B144" s="1" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.3">
@@ -1909,36 +2002,36 @@
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B149" s="1" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B150" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B151" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B152" s="1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B153" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1956,111 +2049,281 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:J12"/>
+  <dimension ref="B2:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:G10"/>
+    <sheetView topLeftCell="A31" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" t="s">
-        <v>143</v>
-      </c>
-      <c r="I6" t="s">
-        <v>144</v>
-      </c>
-      <c r="J6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>139</v>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>